<commit_message>
change in the date of birth
</commit_message>
<xml_diff>
--- a/Dictionary.xlsx
+++ b/Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pabloargote/Dropbox/Columbia/02. Semester/Data_Science/Final project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pabloargote/Documents/GitHub/Final-project-QMSS-GR5069/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>Variable</t>
   </si>
@@ -53,12 +53,6 @@
     <t xml:space="preserve"> country's municipality</t>
   </si>
   <si>
-    <t xml:space="preserve"> year finish high school</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> date of birth</t>
-  </si>
-  <si>
     <t xml:space="preserve"> whether the students works</t>
   </si>
   <si>
@@ -294,6 +288,30 @@
   </si>
   <si>
     <t xml:space="preserve"> employment situation mother: 1 "working" 2 "work ocasionally" 3 "unemployed" 4 "retired" 5 "does not work (sick)" 6 "works in household" 7 "other"</t>
+  </si>
+  <si>
+    <t>year of the exam</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>day of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month of birth </t>
+  </si>
+  <si>
+    <t>year of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> date of birth (day.month.year). Important: it it is possible that some older people took the test that year, because you can take the test as many times as you want.  Most of students should be from 1989</t>
   </si>
 </sst>
 </file>
@@ -617,16 +635,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -639,7 +657,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -647,7 +665,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -655,7 +673,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -663,7 +681,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -671,7 +689,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -679,7 +697,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -687,339 +705,363 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="S19">
         <v>1</v>
       </c>
       <c r="T19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U19">
         <v>2</v>
       </c>
       <c r="V19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="W19">
         <v>3</v>
       </c>
       <c r="X19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y19">
         <v>4</v>
       </c>
       <c r="Z19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="R20">
         <v>5</v>
       </c>
       <c r="S20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="T20">
         <v>6</v>
       </c>
       <c r="U20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V20">
         <v>7</v>
       </c>
       <c r="W20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="X20">
         <v>8</v>
       </c>
       <c r="Y20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z20">
         <v>9</v>
       </c>
       <c r="AA20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q22">
         <v>1</v>
       </c>
       <c r="R22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S22">
         <v>2</v>
       </c>
       <c r="T22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U22">
         <v>3</v>
       </c>
       <c r="V22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W22">
         <v>4</v>
       </c>
       <c r="X22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Y22">
         <v>5</v>
       </c>
       <c r="Z22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AA22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="Q23">
         <v>6</v>
       </c>
       <c r="R23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S23">
         <v>7</v>
       </c>
       <c r="T23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>